<commit_message>
Include more detail in cell parser exception
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheet_examples/test_spreadsheet_bad_types.xlsx
+++ b/src/test/resources/spreadsheet_examples/test_spreadsheet_bad_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.smithchandler/dev/refinery/src/test/resources/spreadsheet_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A4C67C-7135-DA42-9568-6C4B8CC7654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53118A70-AE7C-9946-B112-035A4CB9D438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{870AAEF9-2DE1-494F-88CE-485EB3D1B417}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>string</t>
   </si>
@@ -54,7 +54,7 @@
     <t>optional_str</t>
   </si>
   <si>
-    <t>201/01/2021</t>
+    <t>202/01/2020</t>
   </si>
 </sst>
 </file>
@@ -417,14 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B375211-7F82-3148-A5B5-8DEC9DA19438}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -450,9 +451,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" t="s">
         <v>3</v>
       </c>
@@ -464,10 +463,22 @@
       <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increment col index, remove row
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheet_examples/test_spreadsheet_bad_types.xlsx
+++ b/src/test/resources/spreadsheet_examples/test_spreadsheet_bad_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.smithchandler/dev/refinery/src/test/resources/spreadsheet_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53118A70-AE7C-9946-B112-035A4CB9D438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EBF9E8-C227-6E4E-9368-235DD0F15B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{870AAEF9-2DE1-494F-88CE-485EB3D1B417}"/>
   </bookViews>
@@ -417,68 +417,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B375211-7F82-3148-A5B5-8DEC9DA19438}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>